<commit_message>
BUG-398 Osallistumattomien henkilöiden tietoja ei viedä hakemuspalveluun pistesyötön tuonnissa
</commit_message>
<xml_diff>
--- a/src/test/resources/pistesyotto/pistesyotto.xlsx
+++ b/src/test/resources/pistesyotto/pistesyotto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18820" tabRatio="500"/>
+    <workbookView xWindow="10820" yWindow="3700" windowWidth="25600" windowHeight="18820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1402,10 +1402,10 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1739,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1753,11 +1753,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1766,11 +1766,11 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1779,11 +1779,11 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1803,35 +1803,35 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
@@ -1866,9 +1866,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4">
-        <v>42129</v>
-      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="5" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
silently skip over emptyish (oid,name,hetu,dateofbirth all empty) row
</commit_message>
<xml_diff>
--- a/src/test/resources/pistesyotto/pistesyotto.xlsx
+++ b/src/test/resources/pistesyotto/pistesyotto.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessika/dev/oph/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/pistesyotto/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16420" tabRatio="500"/>
   </bookViews>
@@ -1395,7 +1390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1410,6 +1405,10 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1754,61 +1753,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:J218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
     <col min="3" max="4" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1820,43 +1819,43 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1882,50 +1881,42 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="7"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="5">
-        <v>5</v>
-      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="7"/>
@@ -1940,57 +1931,57 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="7"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
       <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="7"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="5">
-        <v>2</v>
-      </c>
+      <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="7"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>17</v>
@@ -1998,19 +1989,19 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="7"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>17</v>
@@ -2018,19 +2009,19 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="7"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>17</v>
@@ -2038,19 +2029,19 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="7"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>17</v>
@@ -2058,19 +2049,19 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="7"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>17</v>
@@ -2078,19 +2069,19 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="7"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>17</v>
@@ -2098,19 +2089,19 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="7"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>17</v>
@@ -2118,12 +2109,12 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="7"/>
@@ -2138,19 +2129,19 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="7"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>17</v>
@@ -2158,19 +2149,19 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="7"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>17</v>
@@ -2178,19 +2169,19 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="7"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>17</v>
@@ -2198,19 +2189,19 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="7"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>17</v>
@@ -2218,19 +2209,19 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="7"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="5">
-        <v>5.6</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>17</v>
@@ -2238,28 +2229,32 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="7"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="7"/>
@@ -2270,39 +2265,35 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="7"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="5">
-        <v>7</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="7"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>17</v>
@@ -2310,19 +2301,19 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="7"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>17</v>
@@ -2330,12 +2321,12 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="7"/>
@@ -2350,19 +2341,19 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="7"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>17</v>
@@ -2370,19 +2361,19 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="7"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>17</v>
@@ -2390,19 +2381,19 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="7"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>17</v>
@@ -2410,19 +2401,19 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="7"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>17</v>
@@ -2430,57 +2421,57 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="7"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="5"/>
+      <c r="G36" s="5">
+        <v>7</v>
+      </c>
       <c r="H36" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="7"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="5">
-        <v>7</v>
-      </c>
+      <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="7"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>17</v>
@@ -2488,19 +2479,19 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="7"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>17</v>
@@ -2508,19 +2499,19 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="7"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>17</v>
@@ -2528,55 +2519,55 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="7"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="7"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="5">
-        <v>4</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="7"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>17</v>
@@ -2584,19 +2575,19 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="7"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>17</v>
@@ -2604,23 +2595,19 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>17</v>
@@ -2628,30 +2615,36 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
       <c r="H46" s="5" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="7"/>
@@ -2664,21 +2657,17 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5" t="s">
         <v>93</v>
@@ -2686,17 +2675,21 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="E49" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5" t="s">
         <v>93</v>
@@ -2704,21 +2697,17 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5" t="s">
         <v>93</v>
@@ -2726,17 +2715,21 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="7"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="E51" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5" t="s">
         <v>93</v>
@@ -2744,12 +2737,12 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="7"/>
@@ -2762,12 +2755,12 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="7"/>
@@ -2780,12 +2773,12 @@
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="7"/>
@@ -2798,12 +2791,12 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="7"/>
@@ -2816,46 +2809,46 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="7"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="7"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="7"/>
@@ -2868,12 +2861,12 @@
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="7"/>
@@ -2886,12 +2879,12 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="7"/>
@@ -2904,12 +2897,12 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="7"/>
@@ -2922,12 +2915,12 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="7"/>
@@ -2940,12 +2933,12 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="7"/>
@@ -2958,21 +2951,17 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="7"/>
-      <c r="E64" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5" t="s">
         <v>93</v>
@@ -2980,17 +2969,21 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="7"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
+      <c r="E65" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5" t="s">
         <v>93</v>
@@ -2998,12 +2991,12 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="7"/>
@@ -3016,12 +3009,12 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="7"/>
@@ -3034,12 +3027,12 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="7"/>
@@ -3052,12 +3045,12 @@
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="7"/>
@@ -3070,46 +3063,46 @@
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="7"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="7"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10">
       <c r="A72" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="7"/>
@@ -3122,12 +3115,12 @@
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="7"/>
@@ -3140,12 +3133,12 @@
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="7"/>
@@ -3158,12 +3151,12 @@
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="7"/>
@@ -3176,12 +3169,12 @@
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="7"/>
@@ -3194,12 +3187,12 @@
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="7"/>
@@ -3212,12 +3205,12 @@
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="7"/>
@@ -3230,46 +3223,46 @@
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10">
       <c r="A79" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="7"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="7"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10">
       <c r="A81" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="7"/>
@@ -3282,12 +3275,12 @@
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="7"/>
@@ -3300,12 +3293,12 @@
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10">
       <c r="A83" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="7"/>
@@ -3318,21 +3311,17 @@
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10">
       <c r="A84" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="7"/>
-      <c r="E84" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5" t="s">
         <v>93</v>
@@ -3340,17 +3329,21 @@
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10">
       <c r="A85" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
+      <c r="E85" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G85" s="5"/>
       <c r="H85" s="5" t="s">
         <v>93</v>
@@ -3358,12 +3351,12 @@
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10">
       <c r="A86" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="7"/>
@@ -3376,28 +3369,30 @@
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="7"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10">
       <c r="A88" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="7"/>
@@ -3408,30 +3403,28 @@
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10">
       <c r="A89" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="7"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="7"/>
@@ -3444,12 +3437,12 @@
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10">
       <c r="A91" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="7"/>
@@ -3462,12 +3455,12 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10">
       <c r="A92" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="7"/>
@@ -3480,12 +3473,12 @@
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10">
       <c r="A93" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="7"/>
@@ -3498,12 +3491,12 @@
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10">
       <c r="A94" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="7"/>
@@ -3516,12 +3509,12 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10">
       <c r="A95" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="7"/>
@@ -3534,12 +3527,12 @@
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10">
       <c r="A96" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="7"/>
@@ -3552,12 +3545,12 @@
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10">
       <c r="A97" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="7"/>
@@ -3570,12 +3563,12 @@
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10">
       <c r="A98" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="7"/>
@@ -3588,12 +3581,12 @@
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10">
       <c r="A99" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="7"/>
@@ -3606,12 +3599,12 @@
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10">
       <c r="A100" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="7"/>
@@ -3624,12 +3617,12 @@
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10">
       <c r="A101" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="7"/>
@@ -3642,12 +3635,12 @@
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="7"/>
@@ -3660,12 +3653,12 @@
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="7"/>
@@ -3678,12 +3671,12 @@
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10">
       <c r="A104" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="7"/>
@@ -3696,46 +3689,46 @@
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10">
       <c r="A105" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="7"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
-      <c r="H105" s="3"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10">
       <c r="A106" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="7"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10">
       <c r="A107" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="7"/>
@@ -3748,12 +3741,12 @@
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10">
       <c r="A108" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="7"/>
@@ -3766,12 +3759,12 @@
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10">
       <c r="A109" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="7"/>
@@ -3784,12 +3777,12 @@
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10">
       <c r="A110" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="7"/>
@@ -3802,12 +3795,12 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10">
       <c r="A111" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="7"/>
@@ -3820,12 +3813,12 @@
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10">
       <c r="A112" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="7"/>
@@ -3838,12 +3831,12 @@
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10">
       <c r="A113" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="7"/>
@@ -3856,12 +3849,12 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10">
       <c r="A114" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="7"/>
@@ -3874,12 +3867,12 @@
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10">
       <c r="A115" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="7"/>
@@ -3892,12 +3885,12 @@
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10">
       <c r="A116" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="7"/>
@@ -3910,12 +3903,12 @@
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10">
       <c r="A117" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="7"/>
@@ -3928,12 +3921,12 @@
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10">
       <c r="A118" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="7"/>
@@ -3946,21 +3939,17 @@
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10">
       <c r="A119" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="7"/>
-      <c r="E119" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
       <c r="G119" s="5"/>
       <c r="H119" s="5" t="s">
         <v>93</v>
@@ -3968,50 +3957,54 @@
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10">
       <c r="A120" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="7"/>
-      <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="5">
-        <v>6.6</v>
-      </c>
+      <c r="E120" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G120" s="5"/>
       <c r="H120" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10">
       <c r="A121" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="7"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
-      <c r="G121" s="5"/>
+      <c r="G121" s="5">
+        <v>6.6</v>
+      </c>
       <c r="H121" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10">
       <c r="A122" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="7"/>
@@ -4024,12 +4017,12 @@
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10">
       <c r="A123" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="7"/>
@@ -4042,21 +4035,17 @@
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10">
       <c r="A124" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="7"/>
-      <c r="E124" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
       <c r="G124" s="5"/>
       <c r="H124" s="5" t="s">
         <v>93</v>
@@ -4064,17 +4053,21 @@
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10">
       <c r="A125" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="7"/>
-      <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
+      <c r="E125" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G125" s="5"/>
       <c r="H125" s="5" t="s">
         <v>93</v>
@@ -4082,12 +4075,12 @@
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10">
       <c r="A126" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="7"/>
@@ -4100,12 +4093,12 @@
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="7"/>
@@ -4118,12 +4111,12 @@
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10">
       <c r="A128" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C128" s="1"/>
       <c r="D128" s="7"/>
@@ -4136,12 +4129,12 @@
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10">
       <c r="A129" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="7"/>
@@ -4154,12 +4147,12 @@
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10">
       <c r="A130" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="7"/>
@@ -4172,12 +4165,12 @@
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10">
       <c r="A131" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="7"/>
@@ -4190,12 +4183,12 @@
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10">
       <c r="A132" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="7"/>
@@ -4208,12 +4201,12 @@
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10">
       <c r="A133" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="7"/>
@@ -4226,12 +4219,12 @@
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10">
       <c r="A134" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="7"/>
@@ -4244,12 +4237,12 @@
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10">
       <c r="A135" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="7"/>
@@ -4262,12 +4255,12 @@
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10">
       <c r="A136" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="7"/>
@@ -4280,12 +4273,12 @@
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10">
       <c r="A137" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="7"/>
@@ -4298,12 +4291,12 @@
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10">
       <c r="A138" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="7"/>
@@ -4316,12 +4309,12 @@
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10">
       <c r="A139" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="7"/>
@@ -4334,12 +4327,12 @@
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10">
       <c r="A140" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="7"/>
@@ -4352,12 +4345,12 @@
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10">
       <c r="A141" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="7"/>
@@ -4370,12 +4363,12 @@
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10">
       <c r="A142" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="7"/>
@@ -4388,12 +4381,12 @@
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10">
       <c r="A143" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="7"/>
@@ -4406,12 +4399,12 @@
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10">
       <c r="A144" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="7"/>
@@ -4424,12 +4417,12 @@
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10">
       <c r="A145" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="7"/>
@@ -4442,12 +4435,12 @@
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10">
       <c r="A146" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="7"/>
@@ -4460,12 +4453,12 @@
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10">
       <c r="A147" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="7"/>
@@ -4478,21 +4471,17 @@
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10">
       <c r="A148" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="7"/>
-      <c r="E148" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F148" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
       <c r="G148" s="5"/>
       <c r="H148" s="5" t="s">
         <v>93</v>
@@ -4500,17 +4489,21 @@
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10">
       <c r="A149" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="7"/>
-      <c r="E149" s="3"/>
-      <c r="F149" s="3"/>
+      <c r="E149" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F149" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G149" s="5"/>
       <c r="H149" s="5" t="s">
         <v>93</v>
@@ -4518,12 +4511,12 @@
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10">
       <c r="A150" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="7"/>
@@ -4536,12 +4529,12 @@
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10">
       <c r="A151" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="7"/>
@@ -4554,46 +4547,46 @@
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10">
       <c r="A152" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="7"/>
       <c r="E152" s="3"/>
       <c r="F152" s="3"/>
-      <c r="G152" s="3"/>
-      <c r="H152" s="3"/>
+      <c r="G152" s="5"/>
+      <c r="H152" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10">
       <c r="A153" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="7"/>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
-      <c r="G153" s="5"/>
-      <c r="H153" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G153" s="3"/>
+      <c r="H153" s="3"/>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10">
       <c r="A154" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C154" s="1"/>
       <c r="D154" s="7"/>
@@ -4606,46 +4599,46 @@
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10">
       <c r="A155" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="7"/>
       <c r="E155" s="3"/>
       <c r="F155" s="3"/>
-      <c r="G155" s="3"/>
-      <c r="H155" s="3"/>
+      <c r="G155" s="5"/>
+      <c r="H155" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10">
       <c r="A156" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C156" s="1"/>
       <c r="D156" s="7"/>
       <c r="E156" s="3"/>
       <c r="F156" s="3"/>
-      <c r="G156" s="5"/>
-      <c r="H156" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G156" s="3"/>
+      <c r="H156" s="3"/>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10">
       <c r="A157" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="7"/>
@@ -4658,12 +4651,12 @@
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10">
       <c r="A158" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="7"/>
@@ -4676,12 +4669,12 @@
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10">
       <c r="A159" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="7"/>
@@ -4694,12 +4687,12 @@
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10">
       <c r="A160" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C160" s="1"/>
       <c r="D160" s="7"/>
@@ -4712,12 +4705,12 @@
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10">
       <c r="A161" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="7"/>
@@ -4730,12 +4723,12 @@
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10">
       <c r="A162" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="7"/>
@@ -4748,12 +4741,12 @@
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10">
       <c r="A163" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="7"/>
@@ -4766,12 +4759,12 @@
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10">
       <c r="A164" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="7"/>
@@ -4784,12 +4777,12 @@
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10">
       <c r="A165" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="7"/>
@@ -4802,12 +4795,12 @@
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10">
       <c r="A166" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C166" s="1"/>
       <c r="D166" s="7"/>
@@ -4820,21 +4813,17 @@
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10">
       <c r="A167" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C167" s="1"/>
       <c r="D167" s="7"/>
-      <c r="E167" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F167" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
       <c r="G167" s="5"/>
       <c r="H167" s="5" t="s">
         <v>93</v>
@@ -4842,17 +4831,21 @@
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10">
       <c r="A168" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C168" s="1"/>
       <c r="D168" s="7"/>
-      <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
+      <c r="E168" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F168" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G168" s="5"/>
       <c r="H168" s="5" t="s">
         <v>93</v>
@@ -4860,12 +4853,12 @@
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10">
       <c r="A169" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C169" s="1"/>
       <c r="D169" s="7"/>
@@ -4878,12 +4871,12 @@
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10">
       <c r="A170" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C170" s="1"/>
       <c r="D170" s="7"/>
@@ -4896,12 +4889,12 @@
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10">
       <c r="A171" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C171" s="1"/>
       <c r="D171" s="7"/>
@@ -4914,12 +4907,12 @@
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10">
       <c r="A172" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C172" s="1"/>
       <c r="D172" s="7"/>
@@ -4932,12 +4925,12 @@
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10">
       <c r="A173" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C173" s="1"/>
       <c r="D173" s="7"/>
@@ -4950,12 +4943,12 @@
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10">
       <c r="A174" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C174" s="1"/>
       <c r="D174" s="7"/>
@@ -4968,12 +4961,12 @@
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10">
       <c r="A175" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C175" s="1"/>
       <c r="D175" s="7"/>
@@ -4986,55 +4979,51 @@
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10">
       <c r="A176" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C176" s="1"/>
       <c r="D176" s="7"/>
       <c r="E176" s="3"/>
       <c r="F176" s="3"/>
-      <c r="G176" s="3"/>
-      <c r="H176" s="3"/>
+      <c r="G176" s="5"/>
+      <c r="H176" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10">
       <c r="A177" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C177" s="1"/>
       <c r="D177" s="7"/>
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
-      <c r="G177" s="5"/>
-      <c r="H177" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G177" s="3"/>
+      <c r="H177" s="3"/>
       <c r="I177" s="3"/>
       <c r="J177" s="3"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10">
       <c r="A178" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C178" s="1"/>
       <c r="D178" s="7"/>
-      <c r="E178" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F178" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="E178" s="3"/>
+      <c r="F178" s="3"/>
       <c r="G178" s="5"/>
       <c r="H178" s="5" t="s">
         <v>93</v>
@@ -5042,17 +5031,21 @@
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10">
       <c r="A179" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="7"/>
-      <c r="E179" s="3"/>
-      <c r="F179" s="3"/>
+      <c r="E179" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F179" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G179" s="5"/>
       <c r="H179" s="5" t="s">
         <v>93</v>
@@ -5060,12 +5053,12 @@
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10">
       <c r="A180" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C180" s="1"/>
       <c r="D180" s="7"/>
@@ -5078,12 +5071,12 @@
       <c r="I180" s="3"/>
       <c r="J180" s="3"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:10">
       <c r="A181" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C181" s="1"/>
       <c r="D181" s="7"/>
@@ -5096,12 +5089,12 @@
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10">
       <c r="A182" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C182" s="1"/>
       <c r="D182" s="7"/>
@@ -5114,12 +5107,12 @@
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10">
       <c r="A183" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C183" s="1"/>
       <c r="D183" s="7"/>
@@ -5132,12 +5125,12 @@
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10">
       <c r="A184" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C184" s="1"/>
       <c r="D184" s="7"/>
@@ -5150,12 +5143,12 @@
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10">
       <c r="A185" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C185" s="1"/>
       <c r="D185" s="7"/>
@@ -5168,55 +5161,51 @@
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10">
       <c r="A186" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C186" s="1"/>
       <c r="D186" s="7"/>
       <c r="E186" s="3"/>
       <c r="F186" s="3"/>
-      <c r="G186" s="3"/>
-      <c r="H186" s="3"/>
+      <c r="G186" s="5"/>
+      <c r="H186" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10">
       <c r="A187" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="7"/>
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
-      <c r="G187" s="5"/>
-      <c r="H187" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
       <c r="I187" s="3"/>
       <c r="J187" s="3"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10">
       <c r="A188" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="7"/>
-      <c r="E188" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F188" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
       <c r="G188" s="5"/>
       <c r="H188" s="5" t="s">
         <v>93</v>
@@ -5224,17 +5213,21 @@
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10">
       <c r="A189" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="7"/>
-      <c r="E189" s="3"/>
-      <c r="F189" s="3"/>
+      <c r="E189" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F189" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G189" s="5"/>
       <c r="H189" s="5" t="s">
         <v>93</v>
@@ -5242,12 +5235,12 @@
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10">
       <c r="A190" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C190" s="1"/>
       <c r="D190" s="7"/>
@@ -5260,12 +5253,12 @@
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10">
       <c r="A191" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C191" s="1"/>
       <c r="D191" s="7"/>
@@ -5278,12 +5271,12 @@
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10">
       <c r="A192" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="7"/>
@@ -5296,12 +5289,12 @@
       <c r="I192" s="3"/>
       <c r="J192" s="3"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10">
       <c r="A193" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C193" s="1"/>
       <c r="D193" s="7"/>
@@ -5314,12 +5307,12 @@
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10">
       <c r="A194" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="7"/>
@@ -5332,12 +5325,12 @@
       <c r="I194" s="3"/>
       <c r="J194" s="3"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:10">
       <c r="A195" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C195" s="1"/>
       <c r="D195" s="7"/>
@@ -5350,12 +5343,12 @@
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10">
       <c r="A196" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C196" s="1"/>
       <c r="D196" s="7"/>
@@ -5368,12 +5361,12 @@
       <c r="I196" s="3"/>
       <c r="J196" s="3"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10">
       <c r="A197" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="7"/>
@@ -5386,12 +5379,12 @@
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10">
       <c r="A198" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C198" s="1"/>
       <c r="D198" s="7"/>
@@ -5404,12 +5397,12 @@
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10">
       <c r="A199" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="7"/>
@@ -5422,12 +5415,12 @@
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10">
       <c r="A200" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C200" s="1"/>
       <c r="D200" s="7"/>
@@ -5440,12 +5433,12 @@
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10">
       <c r="A201" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="7"/>
@@ -5458,12 +5451,12 @@
       <c r="I201" s="3"/>
       <c r="J201" s="3"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10">
       <c r="A202" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C202" s="1"/>
       <c r="D202" s="7"/>
@@ -5476,12 +5469,12 @@
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10">
       <c r="A203" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C203" s="1"/>
       <c r="D203" s="7"/>
@@ -5494,12 +5487,12 @@
       <c r="I203" s="3"/>
       <c r="J203" s="3"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10">
       <c r="A204" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="7"/>
@@ -5512,12 +5505,12 @@
       <c r="I204" s="3"/>
       <c r="J204" s="3"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10">
       <c r="A205" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C205" s="1"/>
       <c r="D205" s="7"/>
@@ -5530,46 +5523,46 @@
       <c r="I205" s="3"/>
       <c r="J205" s="3"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10">
       <c r="A206" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C206" s="1"/>
       <c r="D206" s="7"/>
       <c r="E206" s="3"/>
       <c r="F206" s="3"/>
-      <c r="G206" s="3"/>
-      <c r="H206" s="3"/>
+      <c r="G206" s="5"/>
+      <c r="H206" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I206" s="3"/>
       <c r="J206" s="3"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10">
       <c r="A207" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C207" s="1"/>
       <c r="D207" s="7"/>
       <c r="E207" s="3"/>
       <c r="F207" s="3"/>
-      <c r="G207" s="5"/>
-      <c r="H207" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G207" s="3"/>
+      <c r="H207" s="3"/>
       <c r="I207" s="3"/>
       <c r="J207" s="3"/>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10">
       <c r="A208" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C208" s="1"/>
       <c r="D208" s="7"/>
@@ -5582,12 +5575,12 @@
       <c r="I208" s="3"/>
       <c r="J208" s="3"/>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:10">
       <c r="A209" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C209" s="1"/>
       <c r="D209" s="7"/>
@@ -5600,80 +5593,80 @@
       <c r="I209" s="3"/>
       <c r="J209" s="3"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:10">
       <c r="A210" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C210" s="1"/>
       <c r="D210" s="7"/>
       <c r="E210" s="3"/>
       <c r="F210" s="3"/>
-      <c r="G210" s="3"/>
-      <c r="H210" s="3"/>
+      <c r="G210" s="5"/>
+      <c r="H210" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I210" s="3"/>
       <c r="J210" s="3"/>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:10">
       <c r="A211" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="7"/>
       <c r="E211" s="3"/>
       <c r="F211" s="3"/>
-      <c r="G211" s="5"/>
-      <c r="H211" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G211" s="3"/>
+      <c r="H211" s="3"/>
       <c r="I211" s="3"/>
       <c r="J211" s="3"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10">
       <c r="A212" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="7"/>
       <c r="E212" s="3"/>
       <c r="F212" s="3"/>
-      <c r="G212" s="3"/>
-      <c r="H212" s="3"/>
+      <c r="G212" s="5"/>
+      <c r="H212" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I212" s="3"/>
       <c r="J212" s="3"/>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:10">
       <c r="A213" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C213" s="1"/>
       <c r="D213" s="7"/>
       <c r="E213" s="3"/>
       <c r="F213" s="3"/>
-      <c r="G213" s="5"/>
-      <c r="H213" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="G213" s="3"/>
+      <c r="H213" s="3"/>
       <c r="I213" s="3"/>
       <c r="J213" s="3"/>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:10">
       <c r="A214" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C214" s="1"/>
       <c r="D214" s="7"/>
@@ -5686,9 +5679,9 @@
       <c r="I214" s="3"/>
       <c r="J214" s="3"/>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:10">
       <c r="A215" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>431</v>
@@ -5704,12 +5697,12 @@
       <c r="I215" s="3"/>
       <c r="J215" s="3"/>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:10">
       <c r="A216" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C216" s="1"/>
       <c r="D216" s="7"/>
@@ -5722,12 +5715,12 @@
       <c r="I216" s="3"/>
       <c r="J216" s="3"/>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:10">
       <c r="A217" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C217" s="1"/>
       <c r="D217" s="7"/>
@@ -5739,6 +5732,24 @@
       </c>
       <c r="I217" s="3"/>
       <c r="J217" s="3"/>
+    </row>
+    <row r="218" spans="1:10">
+      <c r="A218" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C218" s="1"/>
+      <c r="D218" s="7"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="3"/>
+      <c r="G218" s="5"/>
+      <c r="H218" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I218" s="3"/>
+      <c r="J218" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5753,5 +5764,10 @@
     <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>